<commit_message>
Update Group08 DBL-2 Scrum Timesheets 201900131.xlsx
</commit_message>
<xml_diff>
--- a/Group08 DBL-2 Scrum Timesheets 201900131.xlsx
+++ b/Group08 DBL-2 Scrum Timesheets 201900131.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20181751\OneDrive - TU Eindhoven\Documents\GitHub\DBLVis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20183477\Documents\GitHub\DBLVis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D88FE28-B21F-4A62-B829-A4A37472CE3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D827B4-7075-4250-9076-B886361C4DF7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20904" windowHeight="6072" tabRatio="761" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20904" windowHeight="6072" tabRatio="761" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -752,7 +752,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2.2916666666666669E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -805,7 +805,7 @@
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="400337368"/>
@@ -889,7 +889,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2916666666666669E-2</c:v>
+                  <c:v>4.5833333333333337E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1264,10 +1264,10 @@
                 <c:formatCode>[h]:mm</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.9444444444444445E-2</c:v>
+                  <c:v>3.888888888888889E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.472222222222222E-3</c:v>
+                  <c:v>6.9444444444444441E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1373,7 +1373,7 @@
           <a:pPr rtl="0">
             <a:defRPr sz="700"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2239,7 +2239,7 @@
       </c>
       <c r="D6" s="23">
         <f>SUM(Student3!D6,Student1!D6,Student2!D6,Student4!D6,Student5!D6,Student6!D6,Student7!D6,Student8!D6)</f>
-        <v>1.9444444444444445E-2</v>
+        <v>3.888888888888889E-2</v>
       </c>
       <c r="E6" s="23">
         <f>SUM(Student3!E6,Student1!E6,Student2!E6,Student4!E6,Student5!E6,Student6!E6,Student7!E6,Student8!E6)</f>
@@ -2275,11 +2275,11 @@
       </c>
       <c r="M6" s="24">
         <f t="shared" ref="M6:M25" si="0">SUM(C6:L6)</f>
-        <v>1.9444444444444445E-2</v>
+        <v>3.888888888888889E-2</v>
       </c>
       <c r="N6" s="7">
         <f>IF(INDEX(Tasks,1,3)&lt;&gt;"",100*M6/INDEX(Tasks,1,3),"")</f>
-        <v>11.666666666666668</v>
+        <v>23.333333333333336</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="D7" s="17">
         <f>SUM(Student3!D7,Student1!D7,Student2!D7,Student4!D7,Student5!D7,Student6!D7,Student7!D7,Student8!D7)</f>
-        <v>3.472222222222222E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="E7" s="17">
         <f>SUM(Student3!E7,Student1!E7,Student2!E7,Student4!E7,Student5!E7,Student6!E7,Student7!E7,Student8!E7)</f>
@@ -2329,11 +2329,11 @@
       </c>
       <c r="M7" s="25">
         <f t="shared" si="0"/>
-        <v>3.472222222222222E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="N7" s="7">
         <f>IF(INDEX(Tasks,2,3)&lt;&gt;"",100*M7/INDEX(Tasks,2,3),"")</f>
-        <v>1.0416666666666667</v>
+        <v>2.0833333333333335</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
@@ -3504,7 +3504,7 @@
       </c>
       <c r="D34" s="17">
         <f>Student4!D26</f>
-        <v>0</v>
+        <v>2.2916666666666669E-2</v>
       </c>
       <c r="E34" s="17">
         <f>Student4!E26</f>
@@ -3540,7 +3540,7 @@
       </c>
       <c r="M34" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.2916666666666669E-2</v>
       </c>
     </row>
     <row r="35" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3750,7 +3750,7 @@
       </c>
       <c r="D39" s="27">
         <f t="shared" si="2"/>
-        <v>2.2916666666666669E-2</v>
+        <v>4.5833333333333337E-2</v>
       </c>
       <c r="E39" s="27">
         <f t="shared" si="2"/>
@@ -3786,7 +3786,7 @@
       </c>
       <c r="M39" s="27">
         <f t="shared" si="1"/>
-        <v>2.2916666666666669E-2</v>
+        <v>4.5833333333333337E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4380,8 +4380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5538,8 +5538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:Q31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5613,7 +5613,9 @@
         <v>Sprint Planning</v>
       </c>
       <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
+      <c r="D6" s="17">
+        <v>1.9444444444444445E-2</v>
+      </c>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
@@ -5629,7 +5631,9 @@
         <v>Daily Scrum</v>
       </c>
       <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
+      <c r="D7" s="17">
+        <v>3.472222222222222E-3</v>
+      </c>
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
@@ -5934,7 +5938,7 @@
       </c>
       <c r="D26" s="22">
         <f t="shared" ref="D26:L26" si="0">SUM(D6:D25)</f>
-        <v>0</v>
+        <v>2.2916666666666669E-2</v>
       </c>
       <c r="E26" s="22">
         <f t="shared" si="0"/>
@@ -5991,39 +5995,39 @@
       </c>
       <c r="D28" s="18">
         <f>SUM($C$26:D26)</f>
-        <v>0</v>
+        <v>2.2916666666666669E-2</v>
       </c>
       <c r="E28" s="18">
         <f>SUM($C$26:E26)</f>
-        <v>0</v>
+        <v>2.2916666666666669E-2</v>
       </c>
       <c r="F28" s="18">
         <f>SUM($C$26:F26)</f>
-        <v>0</v>
+        <v>2.2916666666666669E-2</v>
       </c>
       <c r="G28" s="18">
         <f>SUM($C$26:G26)</f>
-        <v>0</v>
+        <v>2.2916666666666669E-2</v>
       </c>
       <c r="H28" s="18">
         <f>SUM($C$26:H26)</f>
-        <v>0</v>
+        <v>2.2916666666666669E-2</v>
       </c>
       <c r="I28" s="18">
         <f>SUM($C$26:I26)</f>
-        <v>0</v>
+        <v>2.2916666666666669E-2</v>
       </c>
       <c r="J28" s="18">
         <f>SUM($C$26:J26)</f>
-        <v>0</v>
+        <v>2.2916666666666669E-2</v>
       </c>
       <c r="K28" s="18">
         <f>SUM($C$26:K26)</f>
-        <v>0</v>
+        <v>2.2916666666666669E-2</v>
       </c>
       <c r="L28" s="18">
         <f>SUM($C$26:L26)</f>
-        <v>0</v>
+        <v>2.2916666666666669E-2</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.3">
@@ -6036,39 +6040,39 @@
       </c>
       <c r="D29" s="18">
         <f>Parameters!$G$8-D28</f>
-        <v>5.833333333333333</v>
+        <v>5.8104166666666668</v>
       </c>
       <c r="E29" s="18">
         <f>Parameters!$G$8-E28</f>
-        <v>5.833333333333333</v>
+        <v>5.8104166666666668</v>
       </c>
       <c r="F29" s="18">
         <f>Parameters!$G$8-F28</f>
-        <v>5.833333333333333</v>
+        <v>5.8104166666666668</v>
       </c>
       <c r="G29" s="18">
         <f>Parameters!$G$8-G28</f>
-        <v>5.833333333333333</v>
+        <v>5.8104166666666668</v>
       </c>
       <c r="H29" s="18">
         <f>Parameters!$G$8-H28</f>
-        <v>5.833333333333333</v>
+        <v>5.8104166666666668</v>
       </c>
       <c r="I29" s="18">
         <f>Parameters!$G$8-I28</f>
-        <v>5.833333333333333</v>
+        <v>5.8104166666666668</v>
       </c>
       <c r="J29" s="18">
         <f>Parameters!$G$8-J28</f>
-        <v>5.833333333333333</v>
+        <v>5.8104166666666668</v>
       </c>
       <c r="K29" s="18">
         <f>Parameters!$G$8-K28</f>
-        <v>5.833333333333333</v>
+        <v>5.8104166666666668</v>
       </c>
       <c r="L29" s="18">
         <f>Parameters!$G$8-L28</f>
-        <v>5.833333333333333</v>
+        <v>5.8104166666666668</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
time spent on tasks
</commit_message>
<xml_diff>
--- a/Group08 DBL-2 Scrum Timesheets 201900131.xlsx
+++ b/Group08 DBL-2 Scrum Timesheets 201900131.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/l_petrov_student_tue_nl/Documents/DBLVis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20173771\Documents\GitHub\DBLVis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{2EACCFC8-C5F4-4066-BDC4-D7FC4EE51E5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BA0B23-8F84-45CD-9888-811F6821057A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20904" windowHeight="6072" tabRatio="761" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20904" windowHeight="6072" tabRatio="761" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -288,12 +288,6 @@
     <t>Sprint Tasks</t>
   </si>
   <si>
-    <t>Sprint Task 1.x: Develop Code part</t>
-  </si>
-  <si>
-    <t>Sprint Task 2.x: Develop Report part</t>
-  </si>
-  <si>
     <t>Sprint Task 4.x</t>
   </si>
   <si>
@@ -325,6 +319,12 @@
   </si>
   <si>
     <t>Jay Benedicto</t>
+  </si>
+  <si>
+    <t>Sprint Task 1.1: research javascript, libraries, etc.</t>
+  </si>
+  <si>
+    <t>Sprint Task 1.1: look into data retrieval</t>
   </si>
 </sst>
 </file>
@@ -650,7 +650,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -668,7 +668,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -758,7 +758,7 @@
                   <c:v>2.2916666666666669E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.11666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -805,7 +805,7 @@
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
-            <a:endParaRPr lang="LID4096"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="400337368"/>
@@ -851,7 +851,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -886,10 +886,10 @@
                 <c:formatCode>[h]:mm</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>4.1666666666666664E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.8750000000000006E-2</c:v>
+                  <c:v>0.14374999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -990,7 +990,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1213,10 +1213,10 @@
                   <c:v>Sprint Tasks</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Sprint Task 1.x: Develop Code part</c:v>
+                  <c:v>Sprint Task 1.1: research javascript, libraries, etc.</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Sprint Task 2.x: Develop Report part</c:v>
+                  <c:v>Sprint Task 1.1: look into data retrieval</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Sprint Task 3.x: </c:v>
@@ -1264,10 +1264,10 @@
                 <c:formatCode>[h]:mm</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>5.8333333333333334E-2</c:v>
+                  <c:v>7.7777777777777779E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0416666666666666E-2</c:v>
+                  <c:v>1.3888888888888888E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1276,16 +1276,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4.1666666666666664E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>3.125E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>2.0833333333333332E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1373,7 +1373,7 @@
           <a:pPr rtl="0">
             <a:defRPr sz="700"/>
           </a:pPr>
-          <a:endParaRPr lang="LID4096"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1509,7 +1509,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1835,7 +1835,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1854,7 +1854,7 @@
         <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1885,7 +1885,7 @@
         <v>22</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G5" s="29">
         <v>5.833333333333333</v>
@@ -1905,7 +1905,7 @@
         <v>23</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G6" s="29">
         <v>5.833333333333333</v>
@@ -1925,7 +1925,7 @@
         <v>24</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G7" s="29">
         <v>5.833333333333333</v>
@@ -1945,7 +1945,7 @@
         <v>25</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G8" s="29">
         <v>5.833333333333333</v>
@@ -1965,7 +1965,7 @@
         <v>26</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G9" s="29">
         <v>5.833333333333333</v>
@@ -1985,7 +1985,7 @@
         <v>27</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G10" s="29">
         <v>5.833333333333333</v>
@@ -1996,7 +1996,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="C11" s="28"/>
       <c r="E11" s="15" t="s">
@@ -2012,7 +2012,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="C12" s="28"/>
       <c r="E12" s="15" t="s">
@@ -2028,7 +2028,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C13" s="28"/>
       <c r="F13" s="12" t="s">
@@ -2044,7 +2044,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C14" s="28"/>
     </row>
@@ -2053,7 +2053,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C15" s="28"/>
     </row>
@@ -2062,7 +2062,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C16" s="28"/>
     </row>
@@ -2071,7 +2071,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C17" s="28"/>
     </row>
@@ -2080,7 +2080,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C18" s="28"/>
     </row>
@@ -2089,7 +2089,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C19" s="28"/>
     </row>
@@ -2098,7 +2098,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C20" s="28"/>
     </row>
@@ -2107,7 +2107,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C21" s="28"/>
     </row>
@@ -2116,7 +2116,7 @@
         <v>18</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C22" s="28"/>
     </row>
@@ -2125,7 +2125,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C23" s="28"/>
     </row>
@@ -2134,7 +2134,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C24" s="28"/>
     </row>
@@ -2239,7 +2239,7 @@
       </c>
       <c r="D6" s="23">
         <f>SUM(Student3!D6,Student1!D6,Student2!D6,Student4!D6,Student5!D6,Student6!D6,Student7!D6,Student8!D6)</f>
-        <v>5.8333333333333334E-2</v>
+        <v>7.7777777777777779E-2</v>
       </c>
       <c r="E6" s="23">
         <f>SUM(Student3!E6,Student1!E6,Student2!E6,Student4!E6,Student5!E6,Student6!E6,Student7!E6,Student8!E6)</f>
@@ -2275,11 +2275,11 @@
       </c>
       <c r="M6" s="24">
         <f t="shared" ref="M6:M25" si="0">SUM(C6:L6)</f>
-        <v>5.8333333333333334E-2</v>
+        <v>7.7777777777777779E-2</v>
       </c>
       <c r="N6" s="7">
         <f>IF(INDEX(Tasks,1,3)&lt;&gt;"",100*M6/INDEX(Tasks,1,3),"")</f>
-        <v>35</v>
+        <v>46.666666666666671</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="D7" s="17">
         <f>SUM(Student3!D7,Student1!D7,Student2!D7,Student4!D7,Student5!D7,Student6!D7,Student7!D7,Student8!D7)</f>
-        <v>1.0416666666666666E-2</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="E7" s="17">
         <f>SUM(Student3!E7,Student1!E7,Student2!E7,Student4!E7,Student5!E7,Student6!E7,Student7!E7,Student8!E7)</f>
@@ -2329,11 +2329,11 @@
       </c>
       <c r="M7" s="25">
         <f t="shared" si="0"/>
-        <v>1.0416666666666666E-2</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="N7" s="7">
         <f>IF(INDEX(Tasks,2,3)&lt;&gt;"",100*M7/INDEX(Tasks,2,3),"")</f>
-        <v>3.1249999999999996</v>
+        <v>4.166666666666667</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
@@ -2451,7 +2451,7 @@
       </c>
       <c r="C10" s="17">
         <f>SUM(Student3!C10,Student1!C10,Student2!C10,Student4!C10,Student5!C10,Student6!C10,Student7!C10,Student8!C10)</f>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D10" s="17">
         <f>SUM(Student3!D10,Student1!D10,Student2!D10,Student4!D10,Student5!D10,Student6!D10,Student7!D10,Student8!D10)</f>
@@ -2491,11 +2491,11 @@
       </c>
       <c r="M10" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="N10" s="7">
         <f>IF(INDEX(Tasks,5,3)&lt;&gt;"",100*M10/INDEX(Tasks,5,3),"")</f>
-        <v>0</v>
+        <v>49.999999999999993</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
@@ -2555,7 +2555,7 @@
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
         <f>INDEX(Tasks,7,2)</f>
-        <v>Sprint Task 1.x: Develop Code part</v>
+        <v>Sprint Task 1.1: research javascript, libraries, etc.</v>
       </c>
       <c r="C12" s="17">
         <f>SUM(Student3!C12,Student1!C12,Student2!C12,Student4!C12,Student5!C12,Student6!C12,Student7!C12,Student8!C12)</f>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="D12" s="17">
         <f>SUM(Student3!D12,Student1!D12,Student2!D12,Student4!D12,Student5!D12,Student6!D12,Student7!D12,Student8!D12)</f>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
       <c r="E12" s="17">
         <f>SUM(Student3!E12,Student1!E12,Student2!E12,Student4!E12,Student5!E12,Student6!E12,Student7!E12,Student8!E12)</f>
@@ -2599,7 +2599,7 @@
       </c>
       <c r="M12" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
       <c r="N12" s="7" t="str">
         <f>IF(INDEX(Tasks,7,3)&lt;&gt;"",100*M12/INDEX(Tasks,7,3),"")</f>
@@ -2609,7 +2609,7 @@
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <f>INDEX(Tasks,8,2)</f>
-        <v>Sprint Task 2.x: Develop Report part</v>
+        <v>Sprint Task 1.1: look into data retrieval</v>
       </c>
       <c r="C13" s="17">
         <f>SUM(Student3!C13,Student1!C13,Student2!C13,Student4!C13,Student5!C13,Student6!C13,Student7!C13,Student8!C13)</f>
@@ -2617,7 +2617,7 @@
       </c>
       <c r="D13" s="17">
         <f>SUM(Student3!D13,Student1!D13,Student2!D13,Student4!D13,Student5!D13,Student6!D13,Student7!D13,Student8!D13)</f>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="E13" s="17">
         <f>SUM(Student3!E13,Student1!E13,Student2!E13,Student4!E13,Student5!E13,Student6!E13,Student7!E13,Student8!E13)</f>
@@ -2653,7 +2653,7 @@
       </c>
       <c r="M13" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="N13" s="7" t="str">
         <f>IF(INDEX(Tasks,8,3)&lt;&gt;"",100*M13/INDEX(Tasks,8,3),"")</f>
@@ -3600,11 +3600,11 @@
       </c>
       <c r="C36" s="17">
         <f>Student6!C26</f>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D36" s="17">
         <f>Student6!D26</f>
-        <v>0</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="E36" s="17">
         <f>Student6!E26</f>
@@ -3640,7 +3640,7 @@
       </c>
       <c r="M36" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.11666666666666667</v>
       </c>
     </row>
     <row r="37" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3746,11 +3746,11 @@
     <row r="39" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C39" s="27">
         <f t="shared" ref="C39:L39" si="2">SUM(C31:C38)</f>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D39" s="27">
         <f t="shared" si="2"/>
-        <v>6.8750000000000006E-2</v>
+        <v>0.14374999999999999</v>
       </c>
       <c r="E39" s="27">
         <f t="shared" si="2"/>
@@ -3786,7 +3786,7 @@
       </c>
       <c r="M39" s="27">
         <f t="shared" si="1"/>
-        <v>6.8750000000000006E-2</v>
+        <v>0.18541666666666665</v>
       </c>
     </row>
   </sheetData>
@@ -3803,7 +3803,7 @@
   </sheetPr>
   <dimension ref="A2:Q31"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -3971,7 +3971,7 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
         <f>INDEX(Tasks,7,2)</f>
-        <v>Sprint Task 1.x: Develop Code part</v>
+        <v>Sprint Task 1.1: research javascript, libraries, etc.</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -3987,7 +3987,7 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <f>INDEX(Tasks,8,2)</f>
-        <v>Sprint Task 2.x: Develop Report part</v>
+        <v>Sprint Task 1.1: look into data retrieval</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -4552,7 +4552,7 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
         <f>INDEX(Tasks,7,2)</f>
-        <v>Sprint Task 1.x: Develop Code part</v>
+        <v>Sprint Task 1.1: research javascript, libraries, etc.</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -4568,7 +4568,7 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <f>INDEX(Tasks,8,2)</f>
-        <v>Sprint Task 2.x: Develop Report part</v>
+        <v>Sprint Task 1.1: look into data retrieval</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -5129,7 +5129,7 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
         <f>INDEX(Tasks,7,2)</f>
-        <v>Sprint Task 1.x: Develop Code part</v>
+        <v>Sprint Task 1.1: research javascript, libraries, etc.</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -5145,7 +5145,7 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <f>INDEX(Tasks,8,2)</f>
-        <v>Sprint Task 2.x: Develop Report part</v>
+        <v>Sprint Task 1.1: look into data retrieval</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -5710,7 +5710,7 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
         <f>INDEX(Tasks,7,2)</f>
-        <v>Sprint Task 1.x: Develop Code part</v>
+        <v>Sprint Task 1.1: research javascript, libraries, etc.</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -5726,7 +5726,7 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <f>INDEX(Tasks,8,2)</f>
-        <v>Sprint Task 2.x: Develop Report part</v>
+        <v>Sprint Task 1.1: look into data retrieval</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -6118,7 +6118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -6290,7 +6290,7 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
         <f>INDEX(Tasks,7,2)</f>
-        <v>Sprint Task 1.x: Develop Code part</v>
+        <v>Sprint Task 1.1: research javascript, libraries, etc.</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -6306,7 +6306,7 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <f>INDEX(Tasks,8,2)</f>
-        <v>Sprint Task 2.x: Develop Report part</v>
+        <v>Sprint Task 1.1: look into data retrieval</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -6698,8 +6698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A2:Q31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6773,7 +6773,9 @@
         <v>Sprint Planning</v>
       </c>
       <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
+      <c r="D6" s="17">
+        <v>1.9444444444444445E-2</v>
+      </c>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
@@ -6789,7 +6791,9 @@
         <v>Daily Scrum</v>
       </c>
       <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
+      <c r="D7" s="17">
+        <v>3.472222222222222E-3</v>
+      </c>
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
@@ -6836,7 +6840,9 @@
         <f>INDEX(Tasks,5,2)</f>
         <v>Lectures/Plenary meetings</v>
       </c>
-      <c r="C10" s="17"/>
+      <c r="C10" s="17">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
@@ -6866,10 +6872,12 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
         <f>INDEX(Tasks,7,2)</f>
-        <v>Sprint Task 1.x: Develop Code part</v>
+        <v>Sprint Task 1.1: research javascript, libraries, etc.</v>
       </c>
       <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
+      <c r="D12" s="17">
+        <v>3.125E-2</v>
+      </c>
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
@@ -6882,10 +6890,12 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <f>INDEX(Tasks,8,2)</f>
-        <v>Sprint Task 2.x: Develop Report part</v>
+        <v>Sprint Task 1.1: look into data retrieval</v>
       </c>
       <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
+      <c r="D13" s="17">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
@@ -7090,11 +7100,11 @@
     <row r="26" spans="2:17" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C26" s="22">
         <f>SUM(C6:C25)</f>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D26" s="22">
         <f t="shared" ref="D26:L26" si="0">SUM(D6:D25)</f>
-        <v>0</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="E26" s="22">
         <f t="shared" si="0"/>
@@ -7147,43 +7157,43 @@
       </c>
       <c r="C28" s="18">
         <f>SUM(C26)</f>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D28" s="18">
         <f>SUM($C$26:D26)</f>
-        <v>0</v>
+        <v>0.11666666666666667</v>
       </c>
       <c r="E28" s="18">
         <f>SUM($C$26:E26)</f>
-        <v>0</v>
+        <v>0.11666666666666667</v>
       </c>
       <c r="F28" s="18">
         <f>SUM($C$26:F26)</f>
-        <v>0</v>
+        <v>0.11666666666666667</v>
       </c>
       <c r="G28" s="18">
         <f>SUM($C$26:G26)</f>
-        <v>0</v>
+        <v>0.11666666666666667</v>
       </c>
       <c r="H28" s="18">
         <f>SUM($C$26:H26)</f>
-        <v>0</v>
+        <v>0.11666666666666667</v>
       </c>
       <c r="I28" s="18">
         <f>SUM($C$26:I26)</f>
-        <v>0</v>
+        <v>0.11666666666666667</v>
       </c>
       <c r="J28" s="18">
         <f>SUM($C$26:J26)</f>
-        <v>0</v>
+        <v>0.11666666666666667</v>
       </c>
       <c r="K28" s="18">
         <f>SUM($C$26:K26)</f>
-        <v>0</v>
+        <v>0.11666666666666667</v>
       </c>
       <c r="L28" s="18">
         <f>SUM($C$26:L26)</f>
-        <v>0</v>
+        <v>0.11666666666666667</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.3">
@@ -7192,43 +7202,43 @@
       </c>
       <c r="C29" s="18">
         <f>Parameters!$G$10-C28</f>
-        <v>5.833333333333333</v>
+        <v>5.7916666666666661</v>
       </c>
       <c r="D29" s="18">
         <f>Parameters!$G$10-D28</f>
-        <v>5.833333333333333</v>
+        <v>5.7166666666666668</v>
       </c>
       <c r="E29" s="18">
         <f>Parameters!$G$10-E28</f>
-        <v>5.833333333333333</v>
+        <v>5.7166666666666668</v>
       </c>
       <c r="F29" s="18">
         <f>Parameters!$G$10-F28</f>
-        <v>5.833333333333333</v>
+        <v>5.7166666666666668</v>
       </c>
       <c r="G29" s="18">
         <f>Parameters!$G$10-G28</f>
-        <v>5.833333333333333</v>
+        <v>5.7166666666666668</v>
       </c>
       <c r="H29" s="18">
         <f>Parameters!$G$10-H28</f>
-        <v>5.833333333333333</v>
+        <v>5.7166666666666668</v>
       </c>
       <c r="I29" s="18">
         <f>Parameters!$G$10-I28</f>
-        <v>5.833333333333333</v>
+        <v>5.7166666666666668</v>
       </c>
       <c r="J29" s="18">
         <f>Parameters!$G$10-J28</f>
-        <v>5.833333333333333</v>
+        <v>5.7166666666666668</v>
       </c>
       <c r="K29" s="18">
         <f>Parameters!$G$10-K28</f>
-        <v>5.833333333333333</v>
+        <v>5.7166666666666668</v>
       </c>
       <c r="L29" s="18">
         <f>Parameters!$G$10-L28</f>
-        <v>5.833333333333333</v>
+        <v>5.7166666666666668</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.3">
@@ -7442,7 +7452,7 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
         <f>INDEX(Tasks,7,2)</f>
-        <v>Sprint Task 1.x: Develop Code part</v>
+        <v>Sprint Task 1.1: research javascript, libraries, etc.</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -7458,7 +7468,7 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <f>INDEX(Tasks,8,2)</f>
-        <v>Sprint Task 2.x: Develop Report part</v>
+        <v>Sprint Task 1.1: look into data retrieval</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -8018,7 +8028,7 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
         <f>INDEX(Tasks,7,2)</f>
-        <v>Sprint Task 1.x: Develop Code part</v>
+        <v>Sprint Task 1.1: research javascript, libraries, etc.</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -8034,7 +8044,7 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <f>INDEX(Tasks,8,2)</f>
-        <v>Sprint Task 2.x: Develop Report part</v>
+        <v>Sprint Task 1.1: look into data retrieval</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>

</xml_diff>